<commit_message>
du lieu tot va khong tot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tốt" sheetId="2" r:id="rId2"/>
+    <sheet name="Không tốt" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="419">
   <si>
     <t>Bình luận</t>
   </si>
@@ -332,9 +334,6 @@
     <t>Lỗi camera zalo, không kết thúc cuộc gọi được. Đáng buồn khi mua máy. Không biết bên mình có hỗ trợ đổi mới không, máy mới mua đc 10 ngày</t>
   </si>
   <si>
-    <t>Đt Sài cũng ổn mỗi cái hay bị lỗi Zalo gọi video call tự tắt cam r không kết thúc cuộc gọi được</t>
-  </si>
-  <si>
     <t>máy giật lag,cảm ứng có vẻ không được nhậy</t>
   </si>
   <si>
@@ -542,9 +541,6 @@
     <t>Máy rất lag và sử lý rất chậm, hay bị tuột độ sáng.. không như TGDD quảng cáo. .</t>
   </si>
   <si>
-    <t>essenger không nhận được thông báo cuộc gọi và tin nhắn lỗi tùm lum không hài lòng</t>
-  </si>
-  <si>
     <t>Đt sóng wifi lúc đc lúc ko. Chế độ hậu mãi tệ. TGDD càng ngày càng mất uy tín</t>
   </si>
   <si>
@@ -897,6 +893,396 @@
   </si>
   <si>
     <t>Sạc đầy pin gọi mới mấy cuộc gọi thoại hết pin là sao, mới mua được 1 ngày.,dịch làm sao đổi trả đây</t>
+  </si>
+  <si>
+    <t>Dùng rất tốt</t>
+  </si>
+  <si>
+    <t>quá tốt</t>
+  </si>
+  <si>
+    <t>chất lượng</t>
+  </si>
+  <si>
+    <t>tốt</t>
+  </si>
+  <si>
+    <t>không bị bong</t>
+  </si>
+  <si>
+    <t>Rất thích</t>
+  </si>
+  <si>
+    <t>dễ sữ dụng</t>
+  </si>
+  <si>
+    <t>đẹp</t>
+  </si>
+  <si>
+    <t>bền</t>
+  </si>
+  <si>
+    <t>tuyệt vời</t>
+  </si>
+  <si>
+    <t>tiện dụng</t>
+  </si>
+  <si>
+    <t>hợp lí</t>
+  </si>
+  <si>
+    <t>thời gian bảo hành tốt</t>
+  </si>
+  <si>
+    <t>giá cả hợp lý</t>
+  </si>
+  <si>
+    <t>sử dụng tốt</t>
+  </si>
+  <si>
+    <t>Rất hữu dụng</t>
+  </si>
+  <si>
+    <t>dùng ổn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mượt</t>
+  </si>
+  <si>
+    <t>rất tốt</t>
+  </si>
+  <si>
+    <t>Xài êm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Khá là ổn</t>
+  </si>
+  <si>
+    <t>màu sắc đẹp</t>
+  </si>
+  <si>
+    <t>nhạy</t>
+  </si>
+  <si>
+    <t>máy mượt</t>
+  </si>
+  <si>
+    <t>xử lý tốt</t>
+  </si>
+  <si>
+    <t>xử lí nhanh</t>
+  </si>
+  <si>
+    <t>khỏi phải chê</t>
+  </si>
+  <si>
+    <t>hợp lý</t>
+  </si>
+  <si>
+    <t>ổn định</t>
+  </si>
+  <si>
+    <t>mượt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cực trâu</t>
+  </si>
+  <si>
+    <t>hoàn hảo</t>
+  </si>
+  <si>
+    <t>mượt mà</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> khá ok</t>
+  </si>
+  <si>
+    <t>rất ổn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> khá mượt</t>
+  </si>
+  <si>
+    <t>xài phê</t>
+  </si>
+  <si>
+    <t>rất thích</t>
+  </si>
+  <si>
+    <t>giới thiệu thêm</t>
+  </si>
+  <si>
+    <t>xịn xò</t>
+  </si>
+  <si>
+    <t>Pin khỏe</t>
+  </si>
+  <si>
+    <t>siêu nhanh</t>
+  </si>
+  <si>
+    <t>Ổn Áp</t>
+  </si>
+  <si>
+    <t>nên tham khảo</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>cực nhanh</t>
+  </si>
+  <si>
+    <t>dùng tốt</t>
+  </si>
+  <si>
+    <t>ổn</t>
+  </si>
+  <si>
+    <t>nhẹ</t>
+  </si>
+  <si>
+    <t>suất sắc</t>
+  </si>
+  <si>
+    <t>khá</t>
+  </si>
+  <si>
+    <t>mạnh</t>
+  </si>
+  <si>
+    <t>hay</t>
+  </si>
+  <si>
+    <t>nên mua</t>
+  </si>
+  <si>
+    <t>hài lòng</t>
+  </si>
+  <si>
+    <t>thoải mái</t>
+  </si>
+  <si>
+    <t>Sài ok phết</t>
+  </si>
+  <si>
+    <t>Messenger không nhận được thông báo cuộc gọi và tin nhắn lỗi tùm lum không hài lòng</t>
+  </si>
+  <si>
+    <t>ko mơ gì hơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chắc chắn</t>
+  </si>
+  <si>
+    <t>sóng khỏe</t>
+  </si>
+  <si>
+    <t>tạm ổn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> khá ổn</t>
+  </si>
+  <si>
+    <t>Ngon</t>
+  </si>
+  <si>
+    <t>xứng đáng</t>
+  </si>
+  <si>
+    <t>quá tuyệt</t>
+  </si>
+  <si>
+    <t>sắc nét</t>
+  </si>
+  <si>
+    <t>khỏi bàn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> không bị rè</t>
+  </si>
+  <si>
+    <t>ọp ẹp</t>
+  </si>
+  <si>
+    <t>rất hay</t>
+  </si>
+  <si>
+    <t>rõ ràng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to</t>
+  </si>
+  <si>
+    <t>tiện lợi</t>
+  </si>
+  <si>
+    <t>chán</t>
+  </si>
+  <si>
+    <t>sướng thật</t>
+  </si>
+  <si>
+    <t>thông minh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ăn đứt</t>
+  </si>
+  <si>
+    <t>gọn nhẹ</t>
+  </si>
+  <si>
+    <t>load chậm</t>
+  </si>
+  <si>
+    <t>ko lo hỏng</t>
+  </si>
+  <si>
+    <t>ko giật lag</t>
+  </si>
+  <si>
+    <t>phong phú</t>
+  </si>
+  <si>
+    <t>không nghe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> không hài lòng </t>
+  </si>
+  <si>
+    <t>không được sắc nét</t>
+  </si>
+  <si>
+    <t>không hiểu</t>
+  </si>
+  <si>
+    <t>bực mình</t>
+  </si>
+  <si>
+    <t>độ trễ cao</t>
+  </si>
+  <si>
+    <t>kém</t>
+  </si>
+  <si>
+    <t>hư</t>
+  </si>
+  <si>
+    <t>chậm</t>
+  </si>
+  <si>
+    <t>sai lầm</t>
+  </si>
+  <si>
+    <t>yêu</t>
+  </si>
+  <si>
+    <t>dởm</t>
+  </si>
+  <si>
+    <t>tẩy chay</t>
+  </si>
+  <si>
+    <t>nhanh hết pin</t>
+  </si>
+  <si>
+    <t>thất vọng</t>
+  </si>
+  <si>
+    <t>rất chán</t>
+  </si>
+  <si>
+    <t>hơi nặng</t>
+  </si>
+  <si>
+    <t>Đt Sài cũng ổn mỗi cái hay Ci Zalo gọi video call tự tắt cam r không kết thúc cuộc gọi được</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> giật lag</t>
+  </si>
+  <si>
+    <t>đơ</t>
+  </si>
+  <si>
+    <t>rất khó chịu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tụt ghê</t>
+  </si>
+  <si>
+    <t>rất kém</t>
+  </si>
+  <si>
+    <t>yếu</t>
+  </si>
+  <si>
+    <t>kinh khủng</t>
+  </si>
+  <si>
+    <t>xấu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lỏng lẻo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> không ổn định</t>
+  </si>
+  <si>
+    <t>rất nóng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rất tệ</t>
+  </si>
+  <si>
+    <t>nghe ko được</t>
+  </si>
+  <si>
+    <t>mất uy tín</t>
+  </si>
+  <si>
+    <t>Sai lầm</t>
+  </si>
+  <si>
+    <t>rè rè</t>
+  </si>
+  <si>
+    <t>giao diện rố</t>
+  </si>
+  <si>
+    <t>không nên mua</t>
+  </si>
+  <si>
+    <t>cực kỳ chậm</t>
+  </si>
+  <si>
+    <t>sập nguồn</t>
+  </si>
+  <si>
+    <t>mãi tệ</t>
+  </si>
+  <si>
+    <t>đơ lác</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thấy ghê</t>
+  </si>
+  <si>
+    <t>quá chậm</t>
+  </si>
+  <si>
+    <t>quá ì ạch</t>
+  </si>
+  <si>
+    <t>dễ bị liệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ức chế</t>
+  </si>
+  <si>
+    <t>không cứng cáp</t>
+  </si>
+  <si>
+    <t>đơ lag</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
       <selection activeCell="A300" sqref="A300"/>
     </sheetView>
   </sheetViews>
@@ -2024,7 +2410,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>102</v>
+        <v>389</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
@@ -2032,7 +2418,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
@@ -2040,7 +2426,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
@@ -2048,7 +2434,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
@@ -2056,7 +2442,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
@@ -2064,7 +2450,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
@@ -2072,7 +2458,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
@@ -2080,7 +2466,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B105" t="s">
         <v>5</v>
@@ -2088,7 +2474,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B106" t="s">
         <v>5</v>
@@ -2096,7 +2482,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
@@ -2104,7 +2490,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
@@ -2112,7 +2498,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
@@ -2120,7 +2506,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
@@ -2128,7 +2514,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -2136,7 +2522,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
@@ -2144,7 +2530,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B113" t="s">
         <v>10</v>
@@ -2152,7 +2538,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
@@ -2160,7 +2546,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B115" t="s">
         <v>10</v>
@@ -2168,7 +2554,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B116" t="s">
         <v>10</v>
@@ -2176,7 +2562,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B117" t="s">
         <v>10</v>
@@ -2184,7 +2570,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -2192,7 +2578,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B119" t="s">
         <v>10</v>
@@ -2200,7 +2586,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -2208,7 +2594,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B121" t="s">
         <v>10</v>
@@ -2216,7 +2602,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
@@ -2224,7 +2610,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123" t="s">
         <v>8</v>
@@ -2232,7 +2618,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
@@ -2240,7 +2626,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
@@ -2248,7 +2634,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B126" t="s">
         <v>10</v>
@@ -2256,7 +2642,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B127" t="s">
         <v>8</v>
@@ -2264,7 +2650,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -2272,7 +2658,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -2280,7 +2666,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -2288,7 +2674,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
@@ -2296,7 +2682,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B132" t="s">
         <v>10</v>
@@ -2304,7 +2690,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B133" t="s">
         <v>5</v>
@@ -2312,7 +2698,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
@@ -2320,7 +2706,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B135" t="s">
         <v>10</v>
@@ -2328,7 +2714,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B136" t="s">
         <v>8</v>
@@ -2336,7 +2722,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B137" t="s">
         <v>5</v>
@@ -2344,7 +2730,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B138" t="s">
         <v>8</v>
@@ -2352,7 +2738,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B139" t="s">
         <v>5</v>
@@ -2360,7 +2746,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
@@ -2368,7 +2754,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B141" t="s">
         <v>5</v>
@@ -2376,7 +2762,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B142" t="s">
         <v>10</v>
@@ -2384,7 +2770,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B143" t="s">
         <v>5</v>
@@ -2392,7 +2778,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B144" t="s">
         <v>10</v>
@@ -2400,7 +2786,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
@@ -2408,7 +2794,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B146" t="s">
         <v>5</v>
@@ -2416,7 +2802,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B147" t="s">
         <v>8</v>
@@ -2424,7 +2810,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B148" t="s">
         <v>10</v>
@@ -2432,7 +2818,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B149" t="s">
         <v>8</v>
@@ -2440,7 +2826,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B150" t="s">
         <v>5</v>
@@ -2448,7 +2834,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B151" t="s">
         <v>5</v>
@@ -2456,15 +2842,15 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B152" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B153" t="s">
         <v>5</v>
@@ -2472,7 +2858,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B154" t="s">
         <v>5</v>
@@ -2480,7 +2866,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B155" t="s">
         <v>8</v>
@@ -2488,7 +2874,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B156" t="s">
         <v>5</v>
@@ -2496,7 +2882,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B157" t="s">
         <v>5</v>
@@ -2504,7 +2890,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
@@ -2512,7 +2898,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B159" t="s">
         <v>8</v>
@@ -2520,7 +2906,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
@@ -2528,7 +2914,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
@@ -2536,15 +2922,15 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B162" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
@@ -2552,15 +2938,15 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B164" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
@@ -2568,7 +2954,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
@@ -2576,15 +2962,15 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>172</v>
+        <v>346</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
@@ -2592,7 +2978,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B169" t="s">
         <v>5</v>
@@ -2600,7 +2986,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
@@ -2608,7 +2994,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B171" t="s">
         <v>5</v>
@@ -2616,7 +3002,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
@@ -2624,7 +3010,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B173" t="s">
         <v>5</v>
@@ -2632,7 +3018,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
@@ -2640,7 +3026,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B175" t="s">
         <v>5</v>
@@ -2648,7 +3034,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B176" t="s">
         <v>5</v>
@@ -2656,7 +3042,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B177" t="s">
         <v>5</v>
@@ -2664,7 +3050,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
@@ -2672,7 +3058,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B179" t="s">
         <v>5</v>
@@ -2680,7 +3066,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B180" t="s">
         <v>5</v>
@@ -2688,15 +3074,15 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B181" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B182" t="s">
         <v>8</v>
@@ -2704,7 +3090,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B183" t="s">
         <v>5</v>
@@ -2712,7 +3098,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B184" t="s">
         <v>5</v>
@@ -2720,7 +3106,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B185" t="s">
         <v>5</v>
@@ -2728,7 +3114,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B186" t="s">
         <v>5</v>
@@ -2736,7 +3122,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
@@ -2744,7 +3130,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B188" t="s">
         <v>5</v>
@@ -2752,7 +3138,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B189" t="s">
         <v>8</v>
@@ -2760,7 +3146,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B190" t="s">
         <v>8</v>
@@ -2768,7 +3154,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B191" t="s">
         <v>8</v>
@@ -2776,7 +3162,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B192" t="s">
         <v>5</v>
@@ -2784,7 +3170,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B193" t="s">
         <v>8</v>
@@ -2792,7 +3178,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B194" t="s">
         <v>5</v>
@@ -2800,7 +3186,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B195" t="s">
         <v>8</v>
@@ -2808,7 +3194,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B196" t="s">
         <v>8</v>
@@ -2816,7 +3202,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B197" t="s">
         <v>5</v>
@@ -2824,7 +3210,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B198" t="s">
         <v>5</v>
@@ -2832,7 +3218,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B199" t="s">
         <v>5</v>
@@ -2840,7 +3226,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B200" t="s">
         <v>5</v>
@@ -2848,7 +3234,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
@@ -2856,7 +3242,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B202" t="s">
         <v>5</v>
@@ -2864,7 +3250,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B203" t="s">
         <v>5</v>
@@ -2872,7 +3258,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B204" t="s">
         <v>5</v>
@@ -2880,7 +3266,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B205" t="s">
         <v>8</v>
@@ -2888,7 +3274,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B206" t="s">
         <v>5</v>
@@ -2896,7 +3282,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
@@ -2904,7 +3290,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B208" t="s">
         <v>5</v>
@@ -2912,7 +3298,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B209" t="s">
         <v>5</v>
@@ -2920,7 +3306,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B210" t="s">
         <v>5</v>
@@ -2928,7 +3314,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B211" t="s">
         <v>5</v>
@@ -2936,7 +3322,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B212" t="s">
         <v>10</v>
@@ -2944,7 +3330,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
@@ -2952,7 +3338,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B214" t="s">
         <v>5</v>
@@ -2960,7 +3346,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B215" t="s">
         <v>10</v>
@@ -2968,7 +3354,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
@@ -2976,7 +3362,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B217" t="s">
         <v>8</v>
@@ -2984,7 +3370,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B218" t="s">
         <v>8</v>
@@ -2992,7 +3378,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
@@ -3000,7 +3386,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
@@ -3008,7 +3394,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
@@ -3016,7 +3402,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
@@ -3024,7 +3410,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
@@ -3032,7 +3418,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B224" t="s">
         <v>5</v>
@@ -3040,7 +3426,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B225" t="s">
         <v>5</v>
@@ -3048,7 +3434,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B226" t="s">
         <v>10</v>
@@ -3056,7 +3442,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B227" t="s">
         <v>5</v>
@@ -3064,7 +3450,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B228" t="s">
         <v>5</v>
@@ -3072,7 +3458,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B229" t="s">
         <v>10</v>
@@ -3080,7 +3466,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B230" t="s">
         <v>5</v>
@@ -3088,7 +3474,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B231" t="s">
         <v>5</v>
@@ -3104,7 +3490,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B233" t="s">
         <v>8</v>
@@ -3112,7 +3498,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B234" t="s">
         <v>5</v>
@@ -3120,7 +3506,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B235" t="s">
         <v>5</v>
@@ -3128,7 +3514,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B236" t="s">
         <v>8</v>
@@ -3136,7 +3522,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
@@ -3144,7 +3530,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B238" t="s">
         <v>8</v>
@@ -3152,7 +3538,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B239" t="s">
         <v>8</v>
@@ -3160,7 +3546,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B240" t="s">
         <v>5</v>
@@ -3168,7 +3554,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
@@ -3176,7 +3562,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B242" t="s">
         <v>8</v>
@@ -3184,7 +3570,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B243" t="s">
         <v>10</v>
@@ -3192,7 +3578,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B244" t="s">
         <v>5</v>
@@ -3200,7 +3586,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B245" t="s">
         <v>5</v>
@@ -3208,7 +3594,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B246" t="s">
         <v>5</v>
@@ -3216,15 +3602,15 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B247" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B248" t="s">
         <v>5</v>
@@ -3232,7 +3618,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B249" t="s">
         <v>5</v>
@@ -3240,7 +3626,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B250" t="s">
         <v>8</v>
@@ -3248,7 +3634,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B251" t="s">
         <v>8</v>
@@ -3256,7 +3642,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B252" t="s">
         <v>10</v>
@@ -3264,7 +3650,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B253" t="s">
         <v>5</v>
@@ -3272,7 +3658,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B254" t="s">
         <v>8</v>
@@ -3280,7 +3666,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B255" t="s">
         <v>5</v>
@@ -3288,7 +3674,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B256" t="s">
         <v>5</v>
@@ -3296,7 +3682,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B257" t="s">
         <v>5</v>
@@ -3304,7 +3690,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B258" t="s">
         <v>5</v>
@@ -3312,7 +3698,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B259" t="s">
         <v>5</v>
@@ -3320,7 +3706,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B260" t="s">
         <v>5</v>
@@ -3328,7 +3714,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B261" t="s">
         <v>5</v>
@@ -3336,7 +3722,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B262" t="s">
         <v>5</v>
@@ -3344,7 +3730,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B263" t="s">
         <v>5</v>
@@ -3352,7 +3738,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B264" t="s">
         <v>5</v>
@@ -3360,7 +3746,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B265" t="s">
         <v>5</v>
@@ -3368,7 +3754,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B266" t="s">
         <v>5</v>
@@ -3376,7 +3762,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B267" t="s">
         <v>5</v>
@@ -3384,7 +3770,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B268" t="s">
         <v>8</v>
@@ -3392,7 +3778,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B269" t="s">
         <v>5</v>
@@ -3400,7 +3786,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B270" t="s">
         <v>5</v>
@@ -3408,7 +3794,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B271" t="s">
         <v>5</v>
@@ -3416,7 +3802,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B272" t="s">
         <v>5</v>
@@ -3424,7 +3810,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B273" t="s">
         <v>8</v>
@@ -3432,7 +3818,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B274" t="s">
         <v>8</v>
@@ -3440,7 +3826,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B275" t="s">
         <v>5</v>
@@ -3448,7 +3834,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B276" t="s">
         <v>5</v>
@@ -3456,7 +3842,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B277" t="s">
         <v>5</v>
@@ -3464,7 +3850,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B278" t="s">
         <v>5</v>
@@ -3472,7 +3858,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B279" t="s">
         <v>5</v>
@@ -3480,7 +3866,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B280" t="s">
         <v>5</v>
@@ -3488,7 +3874,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B281" t="s">
         <v>8</v>
@@ -3496,7 +3882,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B282" t="s">
         <v>8</v>
@@ -3504,7 +3890,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B283" t="s">
         <v>8</v>
@@ -3512,7 +3898,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B284" t="s">
         <v>8</v>
@@ -3520,7 +3906,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B285" t="s">
         <v>8</v>
@@ -3528,7 +3914,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B286" t="s">
         <v>8</v>
@@ -3536,7 +3922,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B287" t="s">
         <v>8</v>
@@ -3544,7 +3930,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B288" t="s">
         <v>8</v>
@@ -3552,7 +3938,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B289" t="s">
         <v>8</v>
@@ -3560,7 +3946,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B290" t="s">
         <v>5</v>
@@ -3568,7 +3954,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B291" t="s">
         <v>5</v>
@@ -3576,7 +3962,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B292" t="s">
         <v>8</v>
@@ -3584,7 +3970,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B293" t="s">
         <v>5</v>
@@ -3592,7 +3978,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B294" t="s">
         <v>5</v>
@@ -3600,7 +3986,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B295" t="s">
         <v>5</v>
@@ -3608,7 +3994,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B296" t="s">
         <v>5</v>
@@ -3616,7 +4002,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B297" t="s">
         <v>8</v>
@@ -3624,7 +4010,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B298" t="s">
         <v>5</v>
@@ -3632,7 +4018,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B299" t="s">
         <v>8</v>
@@ -3640,7 +4026,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B300" t="s">
         <v>8</v>
@@ -3650,4 +4036,707 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>371</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A72">
+    <sortCondition ref="A55"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>418</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tien xu ly 300 dong
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="591">
   <si>
     <t>Bình luận</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Trung tâm bảo hành lừa đảo Từ chối bảo hành khách hàng trong khi máy con nguyên tem dữ ốc máy , máy chỉ lỗi pin thay pin là xong , báo khách hàng phải thay main , thay pin tổng 4 triệu 500 nghìn . Từ nay cạch ra …</t>
   </si>
   <si>
-    <t>am sung đã tìm thấy một vàng tại Việt Nam . Thật đơn giản. Một vành này trữ lượng rất lớn trong tương lai</t>
-  </si>
-  <si>
     <t>Sản phẩm tốt, pin trâu, màn hình đẹp, xử lý tốt mình sẽ giới thiệu người thân dùng,</t>
   </si>
   <si>
@@ -688,9 +685,6 @@
     <t>Sản phẩm cực tệ của Nokia .vào mục nào cũng đơ đơ load chậm. Mới trải nghiệm đc 1 ngày mà muốn đổi trả máy</t>
   </si>
   <si>
-    <t>iện thoại mới mua , mà sao thao tác chậm quá , chức năng sữ lý quay lại chậm . chậm hơn cái nokia đời củ , cách đây 10 năm .</t>
-  </si>
-  <si>
     <t>Máy quá chậm, đơ. Danh bạ, cuộc gọi rất chậm. Tôi muốn trả máy. Chính sách đổi trả ra sao.</t>
   </si>
   <si>
@@ -706,12 +700,6 @@
     <t>Điện thoại rất chất lượng. Mình mua ở ĐMX đường 5 BH-ĐH. Nhân viên rất nhiệt tình và dễ thương nha. Mấy chị rất nhiệt tình. Điện thoại rất đẹp, loa lớn, màn hình và cảm ứng okay, mượt và rất ổn trong tầm giá.</t>
   </si>
   <si>
-    <t>ất ok nhé mới mua đây mặc dù là máy cũ chỉ 700k thôi nhưng duyệt web,youtube,chơi một số game nhẹ như đánh bài zombie tsunami ok nhé.nv bán k rành nên cài youtube go rồi quá trời ứng dụng bản go nhưng k cần thiết nhé.đt đủ sức đáp ứng bản thường.loa nghe k lớn lắm nhưng rất trong và hay.pin thì sau 6 tiếng sử dụng.đa số cài ung dụng.cài đặt lại máy.nghe nhạc ít.doc báo.thì hao khoảng 30%.noi chung 700k ok r</t>
-  </si>
-  <si>
-    <t>ất tệ . Đt gọi thì đc nhận cuộc gọi thì bảo đường dây bận . Rồi đi cho nhân viên kiểm tra lại nói là do nhà mạng. Trong khi mình gắn . Mobi . Viettel. Vina. Cả 3 mạng lun đều như vậy. Như 3 sim đó gắn máy khác vẫn Sài bình thường nghe gọi vẫn OK . Ngoài đường thì dịch tgdd thì chỗ mở cửa chổ ko đi vòng vòng mấy chỗ mới có chỗ mở cửa để cho nhân viên coi lại dùm . Mà vẫn vậy thôi có 230k để đó trưng chơi chứ chạy tới chạy lui lỡ gặp chị covi nữa thì khổ</t>
-  </si>
-  <si>
     <t>Ko thua gì 3310 chính hãng . mang riềng là TQ nhưng xài còn hơn chính hãng . quá tuyệt</t>
   </si>
   <si>
@@ -1802,6 +1790,15 @@
   </si>
   <si>
     <t>Vô đối trong tầm giá, hiệu năng mạnh mẽ, thiết kế đẹp, nhân viên TGDĐ hỗ trợ nhiệt tình thân thiện</t>
+  </si>
+  <si>
+    <t>Sam sung đã tìm thấy một vàng tại Việt Nam . Thật đơn giản. Một vành này trữ lượng rất lớn trong tương lai</t>
+  </si>
+  <si>
+    <t>Rất ok nhé mới mua đây mặc dù là máy cũ chỉ 700k thôi nhưng duyệt web,youtube,chơi một số game nhẹ như đánh bài zombie tsunami ok nhé.nv bán k rành nên cài youtube go rồi quá trời ứng dụng bản go nhưng k cần thiết nhé.đt đủ sức đáp ứng bản thường.loa nghe k lớn lắm nhưng rất trong và hay.pin thì sau 6 tiếng sử dụng.đa số cài ung dụng.cài đặt lại máy.nghe nhạc ít.doc báo.thì hao khoảng 30%.noi chung 700k ok r</t>
+  </si>
+  <si>
+    <t>Điện thoại mới mua , mà sao thao tác chậm quá , chức năng sữ lý quay lại chậm . chậm hơn cái nokia đời củ , cách đây 10 năm .</t>
   </si>
 </sst>
 </file>
@@ -2139,15 +2136,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B446"/>
+  <dimension ref="A1:B445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="E407" sqref="E407"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="A224" sqref="A224:XFD224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.59765625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="85" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.19921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2513,7 +2510,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>50</v>
+        <v>588</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -2521,7 +2518,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -2529,7 +2526,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
@@ -2537,7 +2534,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -2545,7 +2542,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -2553,7 +2550,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
         <v>10</v>
@@ -2561,7 +2558,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
@@ -2569,7 +2566,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -2577,7 +2574,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
@@ -2585,7 +2582,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -2593,7 +2590,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
@@ -2601,7 +2598,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
@@ -2609,7 +2606,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -2617,7 +2614,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
@@ -2625,7 +2622,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
         <v>10</v>
@@ -2633,7 +2630,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -2641,7 +2638,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
@@ -2649,7 +2646,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -2657,7 +2654,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -2665,7 +2662,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
@@ -2673,7 +2670,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
@@ -2681,7 +2678,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
@@ -2689,7 +2686,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
@@ -2697,7 +2694,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
@@ -2705,7 +2702,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
@@ -2713,7 +2710,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
@@ -2721,7 +2718,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
@@ -2729,7 +2726,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
@@ -2737,7 +2734,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
@@ -2745,7 +2742,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
@@ -2753,7 +2750,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
@@ -2761,7 +2758,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
@@ -2769,7 +2766,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
@@ -2777,7 +2774,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -2785,7 +2782,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
@@ -2793,7 +2790,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
@@ -2801,7 +2798,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
@@ -2809,7 +2806,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
@@ -2817,7 +2814,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
@@ -2825,7 +2822,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
@@ -2833,7 +2830,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
@@ -2841,7 +2838,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -2849,7 +2846,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
@@ -2857,7 +2854,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
@@ -2865,7 +2862,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
@@ -2873,7 +2870,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
@@ -2881,7 +2878,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
@@ -2889,7 +2886,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
@@ -2897,7 +2894,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B94" t="s">
         <v>10</v>
@@ -2905,7 +2902,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
@@ -2913,7 +2910,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B96" t="s">
         <v>8</v>
@@ -2921,7 +2918,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
@@ -2929,7 +2926,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
@@ -2937,7 +2934,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
@@ -2945,7 +2942,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
@@ -2953,7 +2950,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
@@ -2961,7 +2958,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
@@ -2969,7 +2966,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
@@ -2977,7 +2974,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
@@ -2985,7 +2982,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B105" t="s">
         <v>5</v>
@@ -2993,7 +2990,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
         <v>5</v>
@@ -3001,7 +2998,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
@@ -3009,7 +3006,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
@@ -3017,7 +3014,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
@@ -3025,7 +3022,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
@@ -3033,7 +3030,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -3041,7 +3038,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
@@ -3049,7 +3046,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
         <v>10</v>
@@ -3057,7 +3054,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
@@ -3065,7 +3062,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
         <v>10</v>
@@ -3073,7 +3070,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
         <v>10</v>
@@ -3081,7 +3078,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
         <v>10</v>
@@ -3089,7 +3086,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -3097,7 +3094,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
         <v>10</v>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -3113,7 +3110,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
         <v>10</v>
@@ -3121,7 +3118,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
@@ -3129,7 +3126,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
         <v>8</v>
@@ -3137,7 +3134,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
@@ -3145,7 +3142,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
@@ -3153,7 +3150,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
         <v>10</v>
@@ -3161,7 +3158,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B127" t="s">
         <v>8</v>
@@ -3169,7 +3166,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -3177,7 +3174,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -3185,7 +3182,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -3193,7 +3190,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
@@ -3201,7 +3198,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
         <v>10</v>
@@ -3209,7 +3206,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B133" t="s">
         <v>5</v>
@@ -3217,7 +3214,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
@@ -3225,7 +3222,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B135" t="s">
         <v>10</v>
@@ -3233,7 +3230,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B136" t="s">
         <v>8</v>
@@ -3241,7 +3238,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137" t="s">
         <v>5</v>
@@ -3249,7 +3246,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B138" t="s">
         <v>8</v>
@@ -3257,7 +3254,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B139" t="s">
         <v>5</v>
@@ -3265,7 +3262,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
@@ -3273,7 +3270,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B141" t="s">
         <v>5</v>
@@ -3281,7 +3278,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B142" t="s">
         <v>10</v>
@@ -3289,7 +3286,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B143" t="s">
         <v>5</v>
@@ -3297,7 +3294,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B144" t="s">
         <v>10</v>
@@ -3305,7 +3302,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
@@ -3313,7 +3310,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B146" t="s">
         <v>5</v>
@@ -3321,7 +3318,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B147" t="s">
         <v>8</v>
@@ -3329,7 +3326,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B148" t="s">
         <v>10</v>
@@ -3337,7 +3334,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B149" t="s">
         <v>8</v>
@@ -3345,7 +3342,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B150" t="s">
         <v>5</v>
@@ -3353,7 +3350,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B151" t="s">
         <v>5</v>
@@ -3361,15 +3358,15 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B153" t="s">
         <v>5</v>
@@ -3377,7 +3374,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B154" t="s">
         <v>5</v>
@@ -3385,7 +3382,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B155" t="s">
         <v>8</v>
@@ -3393,7 +3390,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B156" t="s">
         <v>5</v>
@@ -3401,7 +3398,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B157" t="s">
         <v>5</v>
@@ -3409,7 +3406,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B158" t="s">
         <v>8</v>
@@ -3417,7 +3414,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B159" t="s">
         <v>8</v>
@@ -3425,7 +3422,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
@@ -3433,7 +3430,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
@@ -3441,15 +3438,15 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B162" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B163" t="s">
         <v>8</v>
@@ -3457,15 +3454,15 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B164" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
@@ -3473,7 +3470,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
@@ -3481,7 +3478,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
@@ -3489,7 +3486,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
@@ -3497,7 +3494,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B169" t="s">
         <v>5</v>
@@ -3505,7 +3502,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
@@ -3513,7 +3510,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B171" t="s">
         <v>5</v>
@@ -3521,7 +3518,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
@@ -3529,7 +3526,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B173" t="s">
         <v>5</v>
@@ -3537,7 +3534,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
@@ -3545,7 +3542,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B175" t="s">
         <v>5</v>
@@ -3553,7 +3550,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B176" t="s">
         <v>5</v>
@@ -3561,7 +3558,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B177" t="s">
         <v>5</v>
@@ -3569,7 +3566,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
@@ -3577,7 +3574,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B179" t="s">
         <v>5</v>
@@ -3585,7 +3582,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B180" t="s">
         <v>5</v>
@@ -3593,15 +3590,15 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B182" t="s">
         <v>8</v>
@@ -3609,7 +3606,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B183" t="s">
         <v>5</v>
@@ -3617,7 +3614,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B184" t="s">
         <v>5</v>
@@ -3625,7 +3622,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B185" t="s">
         <v>5</v>
@@ -3633,7 +3630,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B186" t="s">
         <v>5</v>
@@ -3641,7 +3638,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
@@ -3649,7 +3646,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B188" t="s">
         <v>5</v>
@@ -3657,7 +3654,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B189" t="s">
         <v>8</v>
@@ -3665,7 +3662,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B190" t="s">
         <v>8</v>
@@ -3673,7 +3670,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B191" t="s">
         <v>8</v>
@@ -3681,7 +3678,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B192" t="s">
         <v>5</v>
@@ -3689,7 +3686,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B193" t="s">
         <v>8</v>
@@ -3697,7 +3694,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B194" t="s">
         <v>5</v>
@@ -3705,7 +3702,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B195" t="s">
         <v>8</v>
@@ -3713,7 +3710,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B196" t="s">
         <v>8</v>
@@ -3721,7 +3718,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B197" t="s">
         <v>5</v>
@@ -3729,7 +3726,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B198" t="s">
         <v>5</v>
@@ -3737,7 +3734,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B199" t="s">
         <v>5</v>
@@ -3745,7 +3742,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B200" t="s">
         <v>5</v>
@@ -3753,7 +3750,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
@@ -3761,7 +3758,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B202" t="s">
         <v>5</v>
@@ -3769,7 +3766,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B203" t="s">
         <v>5</v>
@@ -3777,7 +3774,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B204" t="s">
         <v>5</v>
@@ -3785,7 +3782,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B205" t="s">
         <v>8</v>
@@ -3793,7 +3790,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B206" t="s">
         <v>5</v>
@@ -3801,7 +3798,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B207" t="s">
         <v>8</v>
@@ -3809,7 +3806,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B208" t="s">
         <v>5</v>
@@ -3817,7 +3814,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B209" t="s">
         <v>5</v>
@@ -3825,7 +3822,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B210" t="s">
         <v>5</v>
@@ -3833,7 +3830,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B211" t="s">
         <v>5</v>
@@ -3841,7 +3838,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B212" t="s">
         <v>10</v>
@@ -3849,7 +3846,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B213" t="s">
         <v>8</v>
@@ -3857,7 +3854,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B214" t="s">
         <v>5</v>
@@ -3865,7 +3862,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B215" t="s">
         <v>10</v>
@@ -3873,7 +3870,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B216" t="s">
         <v>8</v>
@@ -3881,7 +3878,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B217" t="s">
         <v>8</v>
@@ -3889,7 +3886,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B218" t="s">
         <v>8</v>
@@ -3897,7 +3894,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B219" t="s">
         <v>8</v>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B220" t="s">
         <v>8</v>
@@ -3913,7 +3910,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B221" t="s">
         <v>8</v>
@@ -3921,7 +3918,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>220</v>
+        <v>590</v>
       </c>
       <c r="B222" t="s">
         <v>8</v>
@@ -3929,7 +3926,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B223" t="s">
         <v>8</v>
@@ -3937,7 +3934,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="B224" t="s">
         <v>5</v>
@@ -3945,18 +3942,18 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B225" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="B226" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -3969,23 +3966,23 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="B228" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B229" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>225</v>
+        <v>589</v>
       </c>
       <c r="B230" t="s">
         <v>5</v>
@@ -3993,7 +3990,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>226</v>
+        <v>5</v>
       </c>
       <c r="B231" t="s">
         <v>5</v>
@@ -4001,23 +3998,23 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="B232" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="B233" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="B234" t="s">
         <v>5</v>
@@ -4025,15 +4022,15 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B235" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B236" t="s">
         <v>8</v>
@@ -4041,7 +4038,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B237" t="s">
         <v>8</v>
@@ -4049,7 +4046,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B238" t="s">
         <v>8</v>
@@ -4057,23 +4054,23 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B239" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B240" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B241" t="s">
         <v>8</v>
@@ -4081,23 +4078,23 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B242" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B243" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B244" t="s">
         <v>5</v>
@@ -4105,7 +4102,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B245" t="s">
         <v>5</v>
@@ -4113,23 +4110,23 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B246" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B247" t="s">
-        <v>161</v>
+        <v>5</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B248" t="s">
         <v>5</v>
@@ -4137,10 +4134,10 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="B249" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -4153,18 +4150,18 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
       <c r="B251" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>243</v>
+        <v>194</v>
       </c>
       <c r="B252" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -4172,20 +4169,20 @@
         <v>195</v>
       </c>
       <c r="B253" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>196</v>
+        <v>240</v>
       </c>
       <c r="B254" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="B255" t="s">
         <v>5</v>
@@ -4193,7 +4190,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
       <c r="B256" t="s">
         <v>5</v>
@@ -4201,7 +4198,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B257" t="s">
         <v>5</v>
@@ -4209,7 +4206,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B258" t="s">
         <v>5</v>
@@ -4217,7 +4214,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B259" t="s">
         <v>5</v>
@@ -4225,7 +4222,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B260" t="s">
         <v>5</v>
@@ -4233,7 +4230,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B261" t="s">
         <v>5</v>
@@ -4241,7 +4238,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B262" t="s">
         <v>5</v>
@@ -4249,7 +4246,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B263" t="s">
         <v>5</v>
@@ -4257,7 +4254,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B264" t="s">
         <v>5</v>
@@ -4265,7 +4262,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B265" t="s">
         <v>5</v>
@@ -4273,7 +4270,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B266" t="s">
         <v>5</v>
@@ -4281,23 +4278,23 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B267" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B268" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B269" t="s">
         <v>5</v>
@@ -4305,7 +4302,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B270" t="s">
         <v>5</v>
@@ -4313,7 +4310,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B271" t="s">
         <v>5</v>
@@ -4321,15 +4318,15 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B272" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B273" t="s">
         <v>8</v>
@@ -4337,15 +4334,15 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B274" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B275" t="s">
         <v>5</v>
@@ -4353,7 +4350,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B276" t="s">
         <v>5</v>
@@ -4361,7 +4358,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B277" t="s">
         <v>5</v>
@@ -4369,7 +4366,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B278" t="s">
         <v>5</v>
@@ -4377,7 +4374,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B279" t="s">
         <v>5</v>
@@ -4385,15 +4382,15 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B280" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B281" t="s">
         <v>8</v>
@@ -4401,7 +4398,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B282" t="s">
         <v>8</v>
@@ -4409,7 +4406,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B283" t="s">
         <v>8</v>
@@ -4417,7 +4414,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B284" t="s">
         <v>8</v>
@@ -4425,7 +4422,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B285" t="s">
         <v>8</v>
@@ -4433,7 +4430,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B286" t="s">
         <v>8</v>
@@ -4441,7 +4438,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B287" t="s">
         <v>8</v>
@@ -4449,7 +4446,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B288" t="s">
         <v>8</v>
@@ -4457,15 +4454,15 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B289" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B290" t="s">
         <v>5</v>
@@ -4473,23 +4470,23 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B291" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B292" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B293" t="s">
         <v>5</v>
@@ -4497,7 +4494,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B294" t="s">
         <v>5</v>
@@ -4505,7 +4502,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B295" t="s">
         <v>5</v>
@@ -4513,31 +4510,31 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B296" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B297" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B298" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B299" t="s">
         <v>8</v>
@@ -4545,7 +4542,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>288</v>
+        <v>415</v>
       </c>
       <c r="B300" t="s">
         <v>8</v>
@@ -4553,7 +4550,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B301" t="s">
         <v>8</v>
@@ -4561,15 +4558,15 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B302" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B303" t="s">
         <v>5</v>
@@ -4577,7 +4574,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B304" t="s">
         <v>5</v>
@@ -4585,7 +4582,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B305" t="s">
         <v>5</v>
@@ -4593,7 +4590,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B306" t="s">
         <v>5</v>
@@ -4601,7 +4598,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B307" t="s">
         <v>5</v>
@@ -4609,7 +4606,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B308" t="s">
         <v>5</v>
@@ -4617,7 +4614,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B309" t="s">
         <v>5</v>
@@ -4625,7 +4622,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B310" t="s">
         <v>5</v>
@@ -4633,7 +4630,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B311" t="s">
         <v>5</v>
@@ -4641,7 +4638,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B312" t="s">
         <v>5</v>
@@ -4649,7 +4646,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B313" t="s">
         <v>5</v>
@@ -4657,7 +4654,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B314" t="s">
         <v>5</v>
@@ -4665,15 +4662,15 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B315" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B316" t="s">
         <v>8</v>
@@ -4681,7 +4678,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B317" t="s">
         <v>8</v>
@@ -4689,7 +4686,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B318" t="s">
         <v>8</v>
@@ -4697,7 +4694,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B319" t="s">
         <v>8</v>
@@ -4705,7 +4702,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B320" t="s">
         <v>8</v>
@@ -4713,7 +4710,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B321" t="s">
         <v>8</v>
@@ -4721,7 +4718,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B322" t="s">
         <v>8</v>
@@ -4729,7 +4726,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B323" t="s">
         <v>8</v>
@@ -4737,7 +4734,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B324" t="s">
         <v>8</v>
@@ -4745,7 +4742,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B325" t="s">
         <v>8</v>
@@ -4753,7 +4750,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B326" t="s">
         <v>8</v>
@@ -4761,7 +4758,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B327" t="s">
         <v>8</v>
@@ -4769,7 +4766,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B328" t="s">
         <v>8</v>
@@ -4777,7 +4774,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B329" t="s">
         <v>8</v>
@@ -4785,7 +4782,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B330" t="s">
         <v>8</v>
@@ -4793,7 +4790,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B331" t="s">
         <v>8</v>
@@ -4801,7 +4798,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B332" t="s">
         <v>8</v>
@@ -4809,7 +4806,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B333" t="s">
         <v>8</v>
@@ -4817,7 +4814,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B334" t="s">
         <v>8</v>
@@ -4825,7 +4822,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B335" t="s">
         <v>8</v>
@@ -4833,7 +4830,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B336" t="s">
         <v>8</v>
@@ -4841,7 +4838,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B337" t="s">
         <v>8</v>
@@ -4849,7 +4846,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B338" t="s">
         <v>8</v>
@@ -4857,7 +4854,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B339" t="s">
         <v>8</v>
@@ -4865,7 +4862,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B340" t="s">
         <v>8</v>
@@ -4873,7 +4870,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B341" t="s">
         <v>8</v>
@@ -4881,7 +4878,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B342" t="s">
         <v>8</v>
@@ -4889,7 +4886,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B343" t="s">
         <v>8</v>
@@ -4897,7 +4894,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B344" t="s">
         <v>8</v>
@@ -4905,7 +4902,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B345" t="s">
         <v>8</v>
@@ -4913,7 +4910,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B346" t="s">
         <v>8</v>
@@ -4921,7 +4918,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B347" t="s">
         <v>8</v>
@@ -4929,7 +4926,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B348" t="s">
         <v>8</v>
@@ -4937,7 +4934,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B349" t="s">
         <v>8</v>
@@ -4945,7 +4942,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B350" t="s">
         <v>8</v>
@@ -4953,7 +4950,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B351" t="s">
         <v>8</v>
@@ -4961,7 +4958,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B352" t="s">
         <v>8</v>
@@ -4969,7 +4966,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B353" t="s">
         <v>8</v>
@@ -4977,7 +4974,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B354" t="s">
         <v>8</v>
@@ -4985,7 +4982,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B355" t="s">
         <v>8</v>
@@ -4993,7 +4990,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B356" t="s">
         <v>8</v>
@@ -5001,7 +4998,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B357" t="s">
         <v>8</v>
@@ -5009,7 +5006,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B358" t="s">
         <v>8</v>
@@ -5017,7 +5014,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B359" t="s">
         <v>8</v>
@@ -5025,7 +5022,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B360" t="s">
         <v>8</v>
@@ -5033,7 +5030,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B361" t="s">
         <v>8</v>
@@ -5041,7 +5038,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B362" t="s">
         <v>8</v>
@@ -5049,7 +5046,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B363" t="s">
         <v>8</v>
@@ -5057,7 +5054,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B364" t="s">
         <v>8</v>
@@ -5065,7 +5062,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B365" t="s">
         <v>8</v>
@@ -5073,7 +5070,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B366" t="s">
         <v>8</v>
@@ -5089,7 +5086,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B368" t="s">
         <v>8</v>
@@ -5097,7 +5094,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B369" t="s">
         <v>8</v>
@@ -5105,7 +5102,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B370" t="s">
         <v>8</v>
@@ -5113,7 +5110,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B371" t="s">
         <v>8</v>
@@ -5121,7 +5118,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B372" t="s">
         <v>8</v>
@@ -5129,7 +5126,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B373" t="s">
         <v>8</v>
@@ -5137,7 +5134,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B374" t="s">
         <v>8</v>
@@ -5145,7 +5142,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B375" t="s">
         <v>8</v>
@@ -5153,7 +5150,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B376" t="s">
         <v>8</v>
@@ -5161,7 +5158,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B377" t="s">
         <v>8</v>
@@ -5169,7 +5166,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B378" t="s">
         <v>8</v>
@@ -5177,7 +5174,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B379" t="s">
         <v>8</v>
@@ -5185,7 +5182,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B380" t="s">
         <v>8</v>
@@ -5193,7 +5190,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B381" t="s">
         <v>8</v>
@@ -5201,7 +5198,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B382" t="s">
         <v>8</v>
@@ -5209,7 +5206,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B383" t="s">
         <v>8</v>
@@ -5217,7 +5214,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B384" t="s">
         <v>8</v>
@@ -5225,7 +5222,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B385" t="s">
         <v>8</v>
@@ -5233,7 +5230,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B386" t="s">
         <v>8</v>
@@ -5241,7 +5238,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B387" t="s">
         <v>8</v>
@@ -5249,7 +5246,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="B388" t="s">
         <v>8</v>
@@ -5257,7 +5254,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B389" t="s">
         <v>8</v>
@@ -5265,7 +5262,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B390" t="s">
         <v>8</v>
@@ -5273,7 +5270,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B391" t="s">
         <v>8</v>
@@ -5281,7 +5278,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B392" t="s">
         <v>8</v>
@@ -5289,7 +5286,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B393" t="s">
         <v>8</v>
@@ -5297,7 +5294,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B394" t="s">
         <v>8</v>
@@ -5305,7 +5302,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B395" t="s">
         <v>8</v>
@@ -5313,7 +5310,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B396" t="s">
         <v>8</v>
@@ -5321,7 +5318,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B397" t="s">
         <v>8</v>
@@ -5329,7 +5326,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B398" t="s">
         <v>8</v>
@@ -5337,7 +5334,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B399" t="s">
         <v>8</v>
@@ -5345,7 +5342,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B400" t="s">
         <v>8</v>
@@ -5353,15 +5350,15 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B401" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B402" t="s">
         <v>5</v>
@@ -5369,7 +5366,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B403" t="s">
         <v>5</v>
@@ -5377,7 +5374,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B404" t="s">
         <v>5</v>
@@ -5385,7 +5382,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B405" t="s">
         <v>5</v>
@@ -5401,7 +5398,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B407" t="s">
         <v>5</v>
@@ -5409,7 +5406,7 @@
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B408" t="s">
         <v>5</v>
@@ -5417,7 +5414,7 @@
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>552</v>
+        <v>425</v>
       </c>
       <c r="B409" t="s">
         <v>5</v>
@@ -5425,7 +5422,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B410" t="s">
         <v>5</v>
@@ -5433,7 +5430,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B411" t="s">
         <v>5</v>
@@ -5441,7 +5438,7 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B412" t="s">
         <v>5</v>
@@ -5449,7 +5446,7 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>433</v>
+        <v>550</v>
       </c>
       <c r="B413" t="s">
         <v>5</v>
@@ -5457,7 +5454,7 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B414" t="s">
         <v>5</v>
@@ -5465,7 +5462,7 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B415" t="s">
         <v>5</v>
@@ -5473,7 +5470,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B416" t="s">
         <v>5</v>
@@ -5481,7 +5478,7 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B417" t="s">
         <v>5</v>
@@ -5489,7 +5486,7 @@
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B418" t="s">
         <v>5</v>
@@ -5497,7 +5494,7 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B419" t="s">
         <v>5</v>
@@ -5505,7 +5502,7 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B420" t="s">
         <v>5</v>
@@ -5513,7 +5510,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B421" t="s">
         <v>5</v>
@@ -5521,7 +5518,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B422" t="s">
         <v>5</v>
@@ -5529,7 +5526,7 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B423" t="s">
         <v>5</v>
@@ -5537,7 +5534,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B424" t="s">
         <v>5</v>
@@ -5545,7 +5542,7 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B425" t="s">
         <v>5</v>
@@ -5553,7 +5550,7 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B426" t="s">
         <v>5</v>
@@ -5561,7 +5558,7 @@
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B427" t="s">
         <v>5</v>
@@ -5569,7 +5566,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B428" t="s">
         <v>5</v>
@@ -5577,7 +5574,7 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B429" t="s">
         <v>5</v>
@@ -5585,7 +5582,7 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B430" t="s">
         <v>5</v>
@@ -5593,7 +5590,7 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B431" t="s">
         <v>5</v>
@@ -5601,7 +5598,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B432" t="s">
         <v>5</v>
@@ -5609,7 +5606,7 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B433" t="s">
         <v>5</v>
@@ -5617,7 +5614,7 @@
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B434" t="s">
         <v>5</v>
@@ -5625,7 +5622,7 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B435" t="s">
         <v>5</v>
@@ -5633,7 +5630,7 @@
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B436" t="s">
         <v>5</v>
@@ -5641,7 +5638,7 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B437" t="s">
         <v>5</v>
@@ -5649,7 +5646,7 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B438" t="s">
         <v>5</v>
@@ -5657,7 +5654,7 @@
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B439" t="s">
         <v>5</v>
@@ -5665,7 +5662,7 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B440" t="s">
         <v>5</v>
@@ -5673,7 +5670,7 @@
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B441" t="s">
         <v>5</v>
@@ -5681,7 +5678,7 @@
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B442" t="s">
         <v>5</v>
@@ -5689,7 +5686,7 @@
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B443" t="s">
         <v>5</v>
@@ -5697,7 +5694,7 @@
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B444" t="s">
         <v>5</v>
@@ -5705,17 +5702,9 @@
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B445" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A446" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="B446" t="s">
         <v>5</v>
       </c>
     </row>
@@ -5737,472 +5726,472 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -6225,377 +6214,377 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>